<commit_message>
[api+front] better parser for charge point excel
</commit_message>
<xml_diff>
--- a/front/public/templates/points-de-recharge-inscription.xlsx
+++ b/front/public/templates/points-de-recharge-inscription.xlsx
@@ -32,7 +32,7 @@
     <t>Date d'installation (ou 01/01/2022 si antérieur)</t>
   </si>
   <si>
-    <t>Numéro LNE du certificat d'examen du type</t>
+    <t>Numéro MID du certificat d'examen du type</t>
   </si>
   <si>
     <t>Date du relevé</t>
@@ -2244,7 +2244,7 @@
     <col min="2" max="3" width="21.5" style="1" customWidth="1"/>
     <col min="4" max="5" width="21.3516" style="1" customWidth="1"/>
     <col min="6" max="6" width="21.5" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.5078" style="1" customWidth="1"/>
+    <col min="7" max="7" width="31.5" style="1" customWidth="1"/>
     <col min="8" max="22" width="12.6719" style="1" customWidth="1"/>
     <col min="23" max="16384" width="12.6719" style="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
chore(elec): specify units in comments next to elec related db columns
</commit_message>
<xml_diff>
--- a/front/public/templates/points-de-recharge-inscription.xlsx
+++ b/front/public/templates/points-de-recharge-inscription.xlsx
@@ -93,7 +93,7 @@
 (ou laisser vide)</t>
   </si>
   <si>
-    <t xml:space="preserve">En W +    <t xml:space="preserve">En kW  (ou laisser vide)</t>
   </si>
   <si>
@@ -176,29 +176,25 @@
   <fonts count="8">
     <font>
       <sz val="10.000000"/>
-      <color indexed="64"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="11.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <sz val="26.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <sz val="16.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
       <sz val="12.000000"/>
-      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
@@ -327,7 +323,7 @@
         <color rgb="FFAAAAAA"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -342,7 +338,7 @@
         <color rgb="FFAAAAAA"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -357,7 +353,7 @@
         <color rgb="FFAAAAAA"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -381,7 +377,7 @@
         <color rgb="FFAAAAAA"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FFAAAAAA"/>
@@ -393,21 +389,21 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
-      <left/>
+      <left style="none"/>
       <right style="thin">
         <color rgb="FFAAAAAA"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -417,7 +413,7 @@
         <color rgb="FFAAAAAA"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color rgb="FFAAAAAA"/>
@@ -432,7 +428,7 @@
         <color rgb="FFA7A7A7"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color rgb="FFAAAAAA"/>
@@ -447,7 +443,7 @@
         <color rgb="FFA7A7A7"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color rgb="FFA7A7A7"/>
@@ -495,7 +491,7 @@
         <color rgb="FFA7A7A7"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -514,27 +510,27 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="none"/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -544,10 +540,10 @@
         <color rgb="FFAAAAAA"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -556,37 +552,37 @@
         <color rgb="FFAAAAAA"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FFAAAAAA"/>
@@ -648,59 +644,59 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -709,25 +705,25 @@
         <color rgb="FFAAAAAA"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FFAAAAAA"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color rgb="FFAAAAAA"/>
@@ -736,235 +732,235 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color rgb="FFAAAAAA"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="none"/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>
@@ -983,13 +979,13 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color rgb="FFAAAAAA"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color rgb="FFAAAAAA"/>
@@ -1001,10 +997,10 @@
         <color rgb="FFAAAAAA"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
         <color rgb="FFAAAAAA"/>
@@ -1044,7 +1040,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
         <color rgb="FFAAAAAA"/>
@@ -1053,7 +1049,7 @@
         <color rgb="FFAAAAAA"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal style="none"/>
     </border>

</xml_diff>